<commit_message>
Correction BACK & Front
</commit_message>
<xml_diff>
--- a/tools/To do-Projet-Mean-M1-P9.xlsx
+++ b/tools/To do-Projet-Mean-M1-P9.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELITEBOOK\Desktop\DAPM\M1\Web-avancé\Projet\m1p9mean-Onjampandresena\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B38C85-D8F4-4EE7-B6BB-1C45E2612549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Ajout collaborateur master1.ituniversity@gmail.com</t>
   </si>
@@ -142,12 +142,15 @@
   </si>
   <si>
     <t xml:space="preserve">Documentation MEAN </t>
+  </si>
+  <si>
+    <t>Learn BACK : CRUD Express and MongoDB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,22 +461,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="65.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="65.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -481,12 +484,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -494,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -502,12 +505,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -515,7 +518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -526,7 +529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -534,7 +537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -542,32 +545,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -578,17 +581,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -596,17 +599,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -614,37 +617,37 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>33</v>
       </c>
@@ -652,14 +655,32 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>